<commit_message>
Działający projekt - plik 123019_Krasniewska_Kamila.qmd
</commit_message>
<xml_diff>
--- a/Dzielnice_Poznan.xlsx
+++ b/Dzielnice_Poznan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60e0003bfb1c8432/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamil\ProjektADN\daneNiekompletneR_V5\mieszkaniaPoznan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="169" documentId="8_{1E965F5D-319D-43F7-9871-CB8E5D70CE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10ADE4B4-55BB-46EC-BE5C-41CE39DA74F2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24B9F35-E058-48C2-B6FD-88716785A031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3F133D20-E7A1-4331-BECC-3067DA22A444}"/>
   </bookViews>
@@ -378,9 +378,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -396,10 +398,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -722,17 +720,17 @@
   <dimension ref="A1:B95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" style="2" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -740,7 +738,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -748,7 +746,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -756,7 +754,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -764,7 +762,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -772,7 +770,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -780,7 +778,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -788,7 +786,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -796,7 +794,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -804,7 +802,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -812,7 +810,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -820,7 +818,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -828,7 +826,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -836,7 +834,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -844,7 +842,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -852,7 +850,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -860,7 +858,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -868,7 +866,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -876,7 +874,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -884,7 +882,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -892,7 +890,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -900,7 +898,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -908,7 +906,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -916,7 +914,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -924,7 +922,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -932,7 +930,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -940,7 +938,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -948,7 +946,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -956,7 +954,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -964,7 +962,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -972,7 +970,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -980,7 +978,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -988,7 +986,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -996,7 +994,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1004,7 +1002,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1012,7 +1010,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1020,7 +1018,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1028,7 +1026,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1036,7 +1034,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -1044,7 +1042,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1052,7 +1050,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1060,7 +1058,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -1068,7 +1066,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -1076,7 +1074,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1084,7 +1082,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1092,7 +1090,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -1100,7 +1098,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -1108,7 +1106,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -1116,7 +1114,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -1124,7 +1122,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -1132,7 +1130,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -1140,7 +1138,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -1148,7 +1146,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -1156,7 +1154,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -1164,7 +1162,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -1172,7 +1170,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -1180,7 +1178,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -1188,7 +1186,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -1196,7 +1194,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -1204,7 +1202,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -1212,7 +1210,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -1220,7 +1218,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -1228,7 +1226,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -1236,7 +1234,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1244,7 +1242,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -1252,7 +1250,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -1260,7 +1258,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -1268,7 +1266,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -1276,7 +1274,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1284,7 +1282,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -1292,7 +1290,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -1300,7 +1298,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -1308,7 +1306,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -1316,7 +1314,7 @@
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -1324,7 +1322,7 @@
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -1332,7 +1330,7 @@
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -1340,7 +1338,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -1348,7 +1346,7 @@
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -1356,7 +1354,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -1364,7 +1362,7 @@
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -1372,7 +1370,7 @@
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B81" s="1" t="s">
@@ -1380,7 +1378,7 @@
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -1388,7 +1386,7 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -1396,7 +1394,7 @@
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -1404,7 +1402,7 @@
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+      <c r="A85" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B85" s="1" t="s">
@@ -1412,7 +1410,7 @@
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -1420,7 +1418,7 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -1428,7 +1426,7 @@
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -1436,7 +1434,7 @@
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B89" s="1" t="s">
@@ -1444,7 +1442,7 @@
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -1452,7 +1450,7 @@
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -1460,7 +1458,7 @@
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
+      <c r="A92" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -1468,7 +1466,7 @@
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
+      <c r="A93" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B93" s="1" t="s">
@@ -1476,7 +1474,7 @@
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
+      <c r="A94" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -1484,7 +1482,7 @@
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="1" t="s">
+      <c r="A95" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B95" s="1" t="s">

</xml_diff>